<commit_message>
Added Armor Part Station w/o functionality and latex documentation
</commit_message>
<xml_diff>
--- a/docs/spreadsheets/oreDistribution.xlsx
+++ b/docs/spreadsheets/oreDistribution.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tudor\Tudor\010_MCM_MinecraftMod\ArmorTinkersMod_1.18.2\docs\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{786D5C78-9945-492A-AAB6-D9C0E691B5DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8884BF1-2FBA-4531-96B2-22FE480BCB37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Distribution" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Distribution!$A$1:$G$1</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="25">
   <si>
     <t>Material</t>
   </si>
@@ -106,7 +109,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -115,19 +118,70 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="20"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -142,10 +196,43 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -430,482 +517,520 @@
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.7109375" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" customWidth="1"/>
-    <col min="6" max="6" width="11" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="14.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" style="1" customWidth="1"/>
+    <col min="4" max="7" width="7.140625" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="12" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2">
+      <c r="C2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="3">
         <v>30</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="3">
         <v>136</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="3">
         <v>256</v>
       </c>
+      <c r="G2" s="3"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3">
+      <c r="A3" s="2"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="3">
         <v>20</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="3">
         <v>0</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="3">
         <v>192</v>
       </c>
+      <c r="G3" s="3"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" t="s">
+      <c r="A4" s="2"/>
+      <c r="B4" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4">
+      <c r="C4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="4">
         <v>90</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="4">
         <v>80</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="4">
         <v>384</v>
       </c>
+      <c r="G4" s="4"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="C5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5">
-        <v>10</v>
-      </c>
-      <c r="E5">
+      <c r="A5" s="2"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="4">
+        <v>10</v>
+      </c>
+      <c r="E5" s="4">
         <v>-24</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="4">
         <v>56</v>
       </c>
+      <c r="G5" s="4"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="C6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6">
-        <v>10</v>
-      </c>
-      <c r="E6">
+      <c r="A6" s="2"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="4">
+        <v>10</v>
+      </c>
+      <c r="E6" s="4">
         <v>-64</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="4">
         <v>72</v>
       </c>
+      <c r="G6" s="4"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" t="s">
+      <c r="A7" s="2"/>
+      <c r="B7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7">
+      <c r="C7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="3">
         <v>16</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="3">
         <v>-16</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="3">
         <v>112</v>
       </c>
+      <c r="G7" s="3"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8">
+      <c r="A8" s="2"/>
+      <c r="B8" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="4">
         <v>4</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="4">
         <v>-64</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="4">
         <v>32</v>
       </c>
+      <c r="G8" s="4"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="C9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9">
+      <c r="A9" s="2"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="4">
         <v>1</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="4">
         <v>-64</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="4">
         <v>-48</v>
       </c>
+      <c r="G9" s="4"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" t="s">
+      <c r="A10" s="2"/>
+      <c r="B10" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10">
-        <v>7</v>
-      </c>
-      <c r="E10">
+      <c r="C10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="3">
+        <v>7</v>
+      </c>
+      <c r="E10" s="3">
         <v>-80</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="3">
         <v>80</v>
       </c>
+      <c r="G10" s="3"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="C11" t="s">
+      <c r="A11" s="2"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="3">
         <v>9</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="3">
         <v>-80</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="3">
         <v>80</v>
       </c>
+      <c r="G11" s="3"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12">
+      <c r="C12" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="6">
         <v>17</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="6">
         <v>-32</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="6">
         <v>80</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="6">
         <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="C13" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13">
-        <v>10</v>
-      </c>
-      <c r="E13">
+      <c r="A13" s="5"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="6">
+        <v>10</v>
+      </c>
+      <c r="E13" s="6">
         <v>-16</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="6">
         <v>112</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="6">
         <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" t="s">
+      <c r="A14" s="5"/>
+      <c r="B14" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C14" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14">
+      <c r="C14" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="7">
         <v>17</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="7">
         <v>-32</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="7">
         <v>80</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="7">
         <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="C15" t="s">
-        <v>7</v>
-      </c>
-      <c r="D15">
-        <v>10</v>
-      </c>
-      <c r="E15">
+      <c r="A15" s="5"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="7">
+        <v>10</v>
+      </c>
+      <c r="E15" s="7">
         <v>-16</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="7">
         <v>112</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="7">
         <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" t="s">
+      <c r="A16" s="5"/>
+      <c r="B16" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16">
-        <v>10</v>
-      </c>
-      <c r="E16">
+      <c r="C16" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="6">
+        <v>10</v>
+      </c>
+      <c r="E16" s="6">
         <v>-40</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="6">
         <v>40</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="6">
         <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="C17" t="s">
-        <v>7</v>
-      </c>
-      <c r="D17">
+      <c r="A17" s="5"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="6">
         <v>15</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="6">
         <v>-64</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="6">
         <v>40</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="6">
         <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" t="s">
+      <c r="A18" s="5"/>
+      <c r="B18" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C18" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18">
-        <v>10</v>
-      </c>
-      <c r="E18">
+      <c r="C18" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="7">
+        <v>10</v>
+      </c>
+      <c r="E18" s="7">
         <v>-40</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="7">
         <v>40</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="7">
         <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="C19" t="s">
-        <v>7</v>
-      </c>
-      <c r="D19">
+      <c r="A19" s="5"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="7">
         <v>15</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="7">
         <v>-64</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="7">
         <v>40</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="7">
         <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="B20" t="s">
+      <c r="A20" s="5"/>
+      <c r="B20" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C20" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20">
-        <v>10</v>
-      </c>
-      <c r="E20">
+      <c r="C20" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="6">
+        <v>10</v>
+      </c>
+      <c r="E20" s="6">
         <v>-80</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="6">
         <v>80</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="6">
         <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
-      <c r="C21" t="s">
-        <v>7</v>
-      </c>
-      <c r="D21">
+      <c r="A21" s="5"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="6">
         <v>30</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="6">
         <v>32</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="6">
         <v>64</v>
       </c>
-      <c r="G21">
+      <c r="G21" s="6">
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-      <c r="B22" t="s">
+    <row r="22" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="5"/>
+      <c r="B22" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C22" t="s">
-        <v>6</v>
-      </c>
-      <c r="D22">
-        <v>10</v>
-      </c>
-      <c r="E22">
+      <c r="C22" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" s="7">
+        <v>10</v>
+      </c>
+      <c r="E22" s="7">
         <v>-80</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="7">
         <v>80</v>
       </c>
-      <c r="G22">
+      <c r="G22" s="7">
         <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-      <c r="C23" t="s">
-        <v>7</v>
-      </c>
-      <c r="D23">
+      <c r="A23" s="5"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" s="7">
         <v>30</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="7">
         <v>-16</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="7">
         <v>16</v>
       </c>
-      <c r="G23">
+      <c r="G23" s="7">
         <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
-      <c r="B24" t="s">
+      <c r="A24" s="5"/>
+      <c r="B24" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C24" t="s">
-        <v>6</v>
-      </c>
-      <c r="D24" t="s">
+      <c r="C24" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E24" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F24" s="6" t="s">
         <v>23</v>
       </c>
+      <c r="G24" s="6" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="1"/>
-      <c r="C25" t="s">
-        <v>7</v>
-      </c>
-      <c r="D25" t="s">
+      <c r="A25" s="5"/>
+      <c r="B25" s="10"/>
+      <c r="C25" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E25" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F25" s="6" t="s">
         <v>23</v>
       </c>
+      <c r="G25" s="6" t="s">
+        <v>23</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="13">
     <mergeCell ref="A2:A11"/>
     <mergeCell ref="A12:A25"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="B24:B25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>